<commit_message>
Water Quality menu content finished
수질 데이터 분석 페이지 모두 완료
</commit_message>
<xml_diff>
--- a/data/rawdata/underground_water.xlsx
+++ b/data/rawdata/underground_water.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63121ca9753f69cb/문서/0.PythonWorkSpace/0.PyCharmProject/Water_project_self/data/rawdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_18BE964F4A06024FD91563D1CC58259495E801D6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B17A4EF-749C-46FF-8880-B0FA96D3BE58}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_18BE964F4A06024FD91563D1CC58259495E801D6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5CD96968-9270-40EB-852D-B259A12EA0BC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2710" yWindow="990" windowWidth="16490" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1774,10 +1774,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -1959,7 +1960,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2404,7 +2405,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2760,7 +2761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2849,7 +2850,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3116,7 +3117,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -3205,7 +3206,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -3294,7 +3295,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -3383,7 +3384,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -3472,7 +3473,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -3561,7 +3562,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3650,7 +3651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -3739,7 +3740,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -3828,7 +3829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3917,7 +3918,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -4006,7 +4007,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -4095,7 +4096,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -4184,7 +4185,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -4273,7 +4274,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -4362,7 +4363,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -4451,7 +4452,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -4629,7 +4630,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -4718,7 +4719,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -4807,7 +4808,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -4896,7 +4897,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -4985,7 +4986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -5074,7 +5075,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -5163,7 +5164,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -5252,7 +5253,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -5341,7 +5342,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -5430,7 +5431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -5519,7 +5520,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -5608,7 +5609,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -5697,7 +5698,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -5786,7 +5787,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -5875,7 +5876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -5964,7 +5965,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -6053,7 +6054,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -6142,7 +6143,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -6231,7 +6232,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -6320,7 +6321,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -6409,7 +6410,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -6498,7 +6499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -6587,7 +6588,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -6676,7 +6677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -6765,7 +6766,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -6854,7 +6855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -6943,7 +6944,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -7032,7 +7033,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -7121,7 +7122,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -7210,7 +7211,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>29</v>
       </c>
@@ -7299,7 +7300,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -7388,7 +7389,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>29</v>
       </c>
@@ -7477,7 +7478,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -7566,7 +7567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -7655,7 +7656,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>29</v>
       </c>
@@ -7744,7 +7745,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>29</v>
       </c>
@@ -7833,7 +7834,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>29</v>
       </c>
@@ -7922,7 +7923,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>29</v>
       </c>
@@ -8011,7 +8012,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>29</v>
       </c>
@@ -8100,7 +8101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>29</v>
       </c>
@@ -8189,7 +8190,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>29</v>
       </c>
@@ -8278,7 +8279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -8367,7 +8368,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -8456,7 +8457,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>29</v>
       </c>
@@ -8545,7 +8546,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>29</v>
       </c>
@@ -8634,7 +8635,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>29</v>
       </c>
@@ -8723,7 +8724,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>29</v>
       </c>
@@ -8812,7 +8813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>29</v>
       </c>
@@ -8901,7 +8902,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>29</v>
       </c>
@@ -8990,7 +8991,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>29</v>
       </c>
@@ -9079,7 +9080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>29</v>
       </c>
@@ -9168,7 +9169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>29</v>
       </c>
@@ -9257,7 +9258,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>29</v>
       </c>
@@ -9346,7 +9347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>29</v>
       </c>
@@ -9435,7 +9436,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -9524,7 +9525,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>29</v>
       </c>
@@ -9613,7 +9614,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>29</v>
       </c>
@@ -9702,7 +9703,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>29</v>
       </c>
@@ -9791,7 +9792,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>29</v>
       </c>
@@ -9880,7 +9881,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>29</v>
       </c>
@@ -9969,7 +9970,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>29</v>
       </c>
@@ -10058,7 +10059,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>29</v>
       </c>
@@ -10147,7 +10148,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>29</v>
       </c>
@@ -10236,7 +10237,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>29</v>
       </c>
@@ -10325,7 +10326,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>29</v>
       </c>
@@ -10414,7 +10415,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>29</v>
       </c>
@@ -10503,7 +10504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>29</v>
       </c>
@@ -10592,7 +10593,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>29</v>
       </c>
@@ -10681,7 +10682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>29</v>
       </c>
@@ -10770,7 +10771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>29</v>
       </c>
@@ -10859,7 +10860,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>29</v>
       </c>
@@ -10948,7 +10949,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>29</v>
       </c>
@@ -11037,7 +11038,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>29</v>
       </c>
@@ -11126,7 +11127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>29</v>
       </c>
@@ -11215,7 +11216,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>29</v>
       </c>
@@ -11304,7 +11305,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>29</v>
       </c>
@@ -11393,7 +11394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>29</v>
       </c>
@@ -11482,7 +11483,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>29</v>
       </c>
@@ -11571,7 +11572,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>29</v>
       </c>
@@ -11660,7 +11661,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>29</v>
       </c>
@@ -11749,7 +11750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>29</v>
       </c>
@@ -11838,7 +11839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>29</v>
       </c>
@@ -11927,7 +11928,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>29</v>
       </c>
@@ -12016,7 +12017,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>29</v>
       </c>
@@ -12105,7 +12106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>29</v>
       </c>
@@ -12194,7 +12195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>29</v>
       </c>
@@ -12283,7 +12284,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>29</v>
       </c>
@@ -12372,7 +12373,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>29</v>
       </c>
@@ -12461,7 +12462,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>29</v>
       </c>
@@ -12550,7 +12551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>29</v>
       </c>
@@ -12639,7 +12640,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>29</v>
       </c>
@@ -12728,7 +12729,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>29</v>
       </c>
@@ -12817,7 +12818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>29</v>
       </c>
@@ -12906,7 +12907,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>29</v>
       </c>
@@ -12995,7 +12996,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>29</v>
       </c>
@@ -13084,7 +13085,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>29</v>
       </c>
@@ -13173,7 +13174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>29</v>
       </c>
@@ -13262,7 +13263,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>29</v>
       </c>
@@ -13351,7 +13352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>29</v>
       </c>
@@ -13440,7 +13441,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>29</v>
       </c>
@@ -13529,7 +13530,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>29</v>
       </c>
@@ -13618,7 +13619,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>29</v>
       </c>
@@ -13707,7 +13708,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>29</v>
       </c>
@@ -13796,7 +13797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>29</v>
       </c>
@@ -13885,7 +13886,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>29</v>
       </c>
@@ -13974,7 +13975,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>29</v>
       </c>
@@ -14063,7 +14064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>29</v>
       </c>
@@ -14152,7 +14153,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>29</v>
       </c>
@@ -14241,7 +14242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>29</v>
       </c>
@@ -14330,7 +14331,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>29</v>
       </c>
@@ -14419,7 +14420,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>29</v>
       </c>
@@ -14508,7 +14509,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>29</v>
       </c>
@@ -14597,7 +14598,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>29</v>
       </c>
@@ -14686,7 +14687,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>29</v>
       </c>
@@ -14775,7 +14776,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>29</v>
       </c>
@@ -14864,7 +14865,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="148" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>29</v>
       </c>
@@ -14953,7 +14954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="149" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>29</v>
       </c>
@@ -15042,7 +15043,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="150" spans="1:29" hidden="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>29</v>
       </c>
@@ -15132,14 +15133,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC150" xr:uid="{B073995E-5C99-4FA8-BD44-0EB945E35E80}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="강정수원"/>
-        <filter val="임원"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AC150" xr:uid="{B073995E-5C99-4FA8-BD44-0EB945E35E80}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>